<commit_message>
Border and Section implemented
</commit_message>
<xml_diff>
--- a/station_in_config/Section.xlsx
+++ b/station_in_config/Section.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="570" windowWidth="11175" windowHeight="8385"/>
+    <workbookView xWindow="13260" yWindow="1560" windowWidth="11175" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,7 +439,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Section and light cells
</commit_message>
<xml_diff>
--- a/station_in_config/Section.xlsx
+++ b/station_in_config/Section.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>name</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>Point_3 Point_14</t>
+  </si>
+  <si>
+    <t>CHP</t>
+  </si>
+  <si>
+    <t>Point_2 Point_9</t>
   </si>
 </sst>
 </file>
@@ -436,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -465,73 +471,81 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>